<commit_message>
marked beers with french characters
</commit_message>
<xml_diff>
--- a/All-About-Beer/data/beer_list.xlsx
+++ b/All-About-Beer/data/beer_list.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DongYi\Documents\GitHub\Beer-Recommendation-App\All-About-Beer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Documents\GitHub\Beer-Recommendation-App\Beer-Recommendation-App\All-About-Beer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCDD8290-0BAF-4172-8DF1-CAEE3D142913}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FA1F70-C361-45F2-A042-657A4D56B0FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DCA9A49-6DBF-4998-A7F7-212516ADAB84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4DCA9A49-6DBF-4998-A7F7-212516ADAB84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$103</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -192,9 +195,6 @@
     <t>'Mill Street Original Organic Lager',</t>
   </si>
   <si>
-    <t>'Tatra Beer',</t>
-  </si>
-  <si>
     <t>'Muskoka Cream Ale',</t>
   </si>
   <si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t xml:space="preserve"> "Kirin Ichiban",</t>
+  </si>
+  <si>
+    <t>Tatra Jasne Pełne / Pils / Beer',</t>
   </si>
 </sst>
 </file>
@@ -355,12 +358,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -375,11 +384,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,560 +707,561 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDE3629-FB58-4BB9-9833-278A3DFC0951}">
   <dimension ref="A1:N103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.26953125" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="1"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="1"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>71</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A90" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A103" xr:uid="{65769BEA-F6EE-4F33-85F0-2A7103052EEC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>